<commit_message>
subtotal iva y total relizados
función subtotal iva y total relizados
</commit_message>
<xml_diff>
--- a/UML/calculo entradas.xlsx
+++ b/UML/calculo entradas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffo\Documents\GitHub\CINE\UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5B1112-2E74-48BA-81A3-7458C4DB1103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876FB613-372F-4404-A3FB-130F4FAE4730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BA23E612-D580-404F-A77A-9D74A27EE4AF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>precio Boleto Cine</t>
   </si>
@@ -77,27 +77,6 @@
   </si>
   <si>
     <t>COSTON*NORMA</t>
-  </si>
-  <si>
-    <t>CALC</t>
-  </si>
-  <si>
-    <t>*0,36</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Adulto</t>
-  </si>
-  <si>
-    <t>Niño</t>
-  </si>
-  <si>
-    <t>3Edad</t>
   </si>
 </sst>
 </file>
@@ -598,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B7C746-025E-4B97-9176-09AA34E758A7}">
-  <dimension ref="B1:Q15"/>
+  <dimension ref="B1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,8 +599,8 @@
     <col min="14" max="14" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
@@ -643,11 +622,8 @@
       <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -662,10 +638,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
         <v>1</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
       </c>
       <c r="I3" s="5">
         <f>C3*D7+C3</f>
@@ -677,43 +653,38 @@
       </c>
       <c r="K3" s="5">
         <f>I3*G3</f>
-        <v>6.0750000000000002</v>
+        <v>0</v>
       </c>
       <c r="L3" s="5">
         <f>H3*J3</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="M3" s="5">
         <f>K3+L3</f>
-        <v>6.0750000000000002</v>
-      </c>
-      <c r="N3" s="5">
-        <f>C3*F3</f>
         <v>4.5</v>
       </c>
+      <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
         <v>12.5</v>
       </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ref="F4:F5" si="0">G4+H4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7">
         <f>(C3/2)*D7+(C3/2)</f>
@@ -725,25 +696,20 @@
       </c>
       <c r="K4" s="7">
         <f>I4*G4</f>
-        <v>6.0750000000000002</v>
+        <v>0</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" ref="L4:L5" si="1">H4*J4</f>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="M4" s="7">
-        <f t="shared" ref="M4:M5" si="2">K4+L4</f>
-        <v>6.0750000000000002</v>
-      </c>
-      <c r="N4" s="7">
-        <f>(C3/2)*F4</f>
-        <v>4.5</v>
-      </c>
+        <f>K4+L4</f>
+        <v>2.25</v>
+      </c>
+      <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="1"/>
       <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
@@ -774,31 +740,12 @@
         <v>2.25</v>
       </c>
       <c r="M5" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M4:M5" si="2">K5+L5</f>
         <v>2.25</v>
       </c>
-      <c r="N5" s="7">
-        <f>(C3/2)*F5</f>
-        <v>2.25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>16</v>
-      </c>
+      <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="N6">
-        <f>SUM(N3:N5)</f>
-        <v>11.25</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <f>P7*N6</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D7">
         <v>0.35</v>
       </c>
@@ -814,17 +761,10 @@
       </c>
       <c r="M7">
         <f>SUM(M3:M5)</f>
-        <v>14.4</v>
-      </c>
-      <c r="N7">
-        <f>N6*D7/6+N6</f>
-        <v>11.90625</v>
-      </c>
-      <c r="P7">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -833,99 +773,19 @@
       </c>
       <c r="M8">
         <f>M7*0.12</f>
-        <v>1.728</v>
-      </c>
-      <c r="N8">
-        <f>N7*0.12</f>
-        <v>1.42875</v>
+        <v>1.08</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>4</v>
+      </c>
       <c r="L9" t="s">
         <v>9</v>
       </c>
       <c r="M9">
         <f>M7+M8</f>
-        <v>16.128</v>
-      </c>
-      <c r="N9">
-        <f>N7+N8</f>
-        <v>13.335000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="J11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
-      <c r="J12">
-        <v>3</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12">
-        <f>F12*(C3*0.35+C3)</f>
-        <v>6.0750000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="L13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13">
-        <f>G12*(C3/2*0.35+C3/2)</f>
-        <v>6.0750000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="L14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14">
-        <f>H12*(C3/2)</f>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="M15">
-        <f>SUM(M12:M14)</f>
-        <v>14.4</v>
-      </c>
-      <c r="O15">
-        <f>J12*0.35</f>
-        <v>1.0499999999999998</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
+        <v>10.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>